<commit_message>
add some more defaults and more units, make a start on converstion between mol and g
</commit_message>
<xml_diff>
--- a/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
+++ b/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64562B-6DE5-4278-9F66-B66EA229C393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DF63A9-16F2-4301-BF26-A0395729B774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6290" yWindow="4530" windowWidth="21820" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cmpt_PK_Model" sheetId="1" r:id="rId1"/>
     <sheet name="2cmpt_PK_Model" sheetId="3" r:id="rId2"/>
     <sheet name="3cmpt_PK_Model" sheetId="4" r:id="rId3"/>
     <sheet name="1cmpt_TMDD_Model" sheetId="5" r:id="rId4"/>
+    <sheet name="2cmpt_TMDD_Model" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="41">
   <si>
     <t>SM_Mouse</t>
   </si>
@@ -174,7 +175,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +208,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +252,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -234,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,6 +285,12 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2691,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3512,6 +3557,905 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D461711-106C-4DEE-9CBC-A04E17BA8C3A}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="14">
+        <v>0</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="14">
+        <v>1</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="14">
+        <v>40</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="14">
+        <v>40</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="14">
+        <v>2</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="14">
+        <v>40</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="14">
+        <v>150</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="14">
+        <v>3000</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14">
+        <v>40</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14">
+        <v>2</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="14">
+        <v>40</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="14">
+        <v>2</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="14">
+        <v>40</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="14">
+        <v>150</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="14">
+        <v>3000</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="14">
+        <v>540</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="14">
+        <v>330</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="14">
+        <v>260</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="14">
+        <v>10</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="14">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2700</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1.8</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1650</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="14">
+        <v>1300</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="14">
+        <v>50</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="14">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="14">
+        <v>1</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="14">
+        <v>1</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="14">
+        <v>1</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.69314718099999995</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="14">
+        <v>0.69314718099999995</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="14">
+        <v>0.69314718099999995</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="14">
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="14">
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="14">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="14">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="14">
+        <v>2.0712917000000001E-2</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="14">
+        <v>2.0712917000000001E-2</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="14">
+        <v>9.6299999999999997E-3</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="14">
+        <v>9.6299999999999997E-3</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.103564586</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="14">
+        <v>0.103564586</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="14">
+        <v>4.8140000000000002E-2</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="14">
+        <v>4.8140000000000002E-2</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update default parameters and make variables in tmdd models consistent
</commit_message>
<xml_diff>
--- a/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
+++ b/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DF63A9-16F2-4301-BF26-A0395729B774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C9D9F0-B865-4D27-A6F1-FA4A16C13C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8030" yWindow="3350" windowWidth="28800" windowHeight="15370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cmpt_PK_Model" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="41">
   <si>
     <t>SM_Mouse</t>
   </si>
@@ -159,10 +159,10 @@
     <t>kint</t>
   </si>
   <si>
-    <t>KD</t>
+    <t>KSS</t>
   </si>
   <si>
-    <t>KSS</t>
+    <t>KD</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,40 +208,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,12 +220,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -273,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,12 +247,6 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +530,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="B3" sqref="B3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,49 +960,49 @@
         <v>31</v>
       </c>
       <c r="B9" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H9" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J9" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="L9" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N9" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="P9" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>33</v>
@@ -1057,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
@@ -1069,7 +1025,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>15</v>
@@ -1081,7 +1037,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>15</v>
@@ -1093,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="N10" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>15</v>
@@ -1110,7 +1066,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
@@ -1122,7 +1078,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>29</v>
@@ -1134,7 +1090,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>29</v>
@@ -1146,7 +1102,7 @@
         <v>29</v>
       </c>
       <c r="N11" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>29</v>
@@ -1169,7 +1125,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1488,14 +1444,14 @@
         <f>B6</f>
         <v>2</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q7" si="0">C6</f>
         <v>L/kg</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -1503,7 +1459,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L/kg</v>
       </c>
@@ -1511,7 +1467,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -1519,7 +1475,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L/kg</v>
       </c>
@@ -1527,7 +1483,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -1535,14 +1491,14 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="P7" s="5">
         <v>3000</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="Q7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL</v>
       </c>
@@ -1616,7 +1572,7 @@
         <f>B8*5</f>
         <v>2700</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="3" t="str">
         <f t="shared" ref="C9:Q9" si="1">C8</f>
         <v>mL/h/kg</v>
       </c>
@@ -1624,7 +1580,7 @@
         <f>D8*5</f>
         <v>1.75</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -1632,7 +1588,7 @@
         <f>F8*5</f>
         <v>1650</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -1640,7 +1596,7 @@
         <f>H8*5</f>
         <v>2</v>
       </c>
-      <c r="I9" t="str">
+      <c r="I9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -1648,7 +1604,7 @@
         <f>J8*5</f>
         <v>1300</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -1656,7 +1612,7 @@
         <f>L8*5</f>
         <v>1.25</v>
       </c>
-      <c r="M9" t="str">
+      <c r="M9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -1664,7 +1620,7 @@
         <f>N8*5</f>
         <v>50</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L/h</v>
       </c>
@@ -1672,7 +1628,7 @@
         <f>P8*5</f>
         <v>40</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="Q9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h</v>
       </c>
@@ -1743,49 +1699,49 @@
         <v>31</v>
       </c>
       <c r="B11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="L11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="P11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>33</v>
@@ -1795,49 +1751,49 @@
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5">
         <v>0.1</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5">
         <v>0.1</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="5">
         <v>0.1</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0.1</v>
-      </c>
       <c r="M12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="6">
-        <v>0.1</v>
+      <c r="N12" s="5">
+        <v>0.5</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="5">
         <v>0.1</v>
       </c>
       <c r="Q12" s="3" t="s">
@@ -1849,7 +1805,7 @@
         <v>32</v>
       </c>
       <c r="B13" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>29</v>
@@ -1861,19 +1817,19 @@
         <v>29</v>
       </c>
       <c r="F13" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>0.2</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="J13" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>29</v>
@@ -1885,7 +1841,7 @@
         <v>29</v>
       </c>
       <c r="N13" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>29</v>
@@ -1908,7 +1864,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:E29"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2226,14 +2182,14 @@
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q8" si="0">C6</f>
         <v>L/kg</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -2241,7 +2197,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L/kg</v>
       </c>
@@ -2249,7 +2205,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -2257,7 +2213,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L/kg</v>
       </c>
@@ -2265,7 +2221,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL/kg</v>
       </c>
@@ -2273,14 +2229,14 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="P7" s="5">
         <v>3000</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="Q7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mL</v>
       </c>
@@ -2293,7 +2249,7 @@
         <f>B7/2</f>
         <v>1</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L/kg</v>
       </c>
@@ -2301,30 +2257,50 @@
         <f>D7/2</f>
         <v>20</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="3" t="str">
         <f>E7</f>
         <v>mL/kg</v>
       </c>
       <c r="F8" s="5">
         <f>F7/2</f>
         <v>1</v>
+      </c>
+      <c r="G8" s="3" t="str">
+        <f>G7</f>
+        <v>L/kg</v>
       </c>
       <c r="H8" s="5">
         <f>H7/2</f>
         <v>20</v>
       </c>
-      <c r="J8" s="5">
+      <c r="I8" s="3" t="str">
+        <f>I7</f>
+        <v>mL/kg</v>
+      </c>
+      <c r="J8" s="7">
         <f>J7/2</f>
         <v>1</v>
       </c>
-      <c r="L8" s="5">
+      <c r="K8" s="3" t="str">
+        <f>K7</f>
+        <v>L/kg</v>
+      </c>
+      <c r="L8" s="8">
         <f>L7/2</f>
         <v>20</v>
+      </c>
+      <c r="M8" s="3" t="str">
+        <f>M7</f>
+        <v>mL/kg</v>
       </c>
       <c r="N8" s="5">
         <f>N7/2</f>
         <v>75</v>
       </c>
+      <c r="O8" s="3" t="str">
+        <f>O7</f>
+        <v>L</v>
+      </c>
       <c r="P8" s="5">
         <f>P7/2</f>
         <v>1500</v>
@@ -2402,7 +2378,7 @@
         <f>B9*5</f>
         <v>2700</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="3" t="str">
         <f t="shared" ref="C10:Q11" si="1">C9</f>
         <v>mL/h/kg</v>
       </c>
@@ -2410,7 +2386,7 @@
         <f>D9*5</f>
         <v>1.75</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2418,7 +2394,7 @@
         <f>F9*5</f>
         <v>1650</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2426,7 +2402,7 @@
         <f>H9*5</f>
         <v>2</v>
       </c>
-      <c r="I10" t="str">
+      <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2434,7 +2410,7 @@
         <f>J9*5</f>
         <v>1300</v>
       </c>
-      <c r="K10" t="str">
+      <c r="K10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2442,7 +2418,7 @@
         <f>L9*5</f>
         <v>1.25</v>
       </c>
-      <c r="M10" t="str">
+      <c r="M10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2450,7 +2426,7 @@
         <f>N9*5</f>
         <v>50</v>
       </c>
-      <c r="O10" t="str">
+      <c r="O10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L/h</v>
       </c>
@@ -2458,7 +2434,7 @@
         <f>P9*5</f>
         <v>40</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="Q10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h</v>
       </c>
@@ -2471,7 +2447,7 @@
         <f>B10/50</f>
         <v>54</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>mL/h/kg</v>
       </c>
@@ -2479,34 +2455,58 @@
         <f>D10/50</f>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="3" t="str">
         <f>E10</f>
         <v>mL/h/kg</v>
       </c>
       <c r="F11" s="5">
         <f>F10/50</f>
         <v>33</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
       </c>
       <c r="H11" s="5">
         <f>H10/50</f>
         <v>0.04</v>
       </c>
+      <c r="I11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
       <c r="J11" s="5">
         <f>J10/50</f>
         <v>26</v>
       </c>
+      <c r="K11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
       <c r="L11" s="5">
         <f>L10/50</f>
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="M11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
       <c r="N11" s="5">
         <f>N10/50</f>
         <v>1</v>
+      </c>
+      <c r="O11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>L/h</v>
       </c>
       <c r="P11" s="5">
         <f>P10/50</f>
         <v>0.8</v>
       </c>
+      <c r="Q11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -2574,49 +2574,49 @@
         <v>31</v>
       </c>
       <c r="B13" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H13" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J13" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="L13" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N13" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="P13" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>33</v>
@@ -2626,49 +2626,49 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5">
         <v>0.1</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="5">
         <v>0.1</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="5">
         <v>0.1</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0.1</v>
-      </c>
       <c r="M14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="6">
-        <v>0.1</v>
+      <c r="N14" s="5">
+        <v>0.5</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="5">
         <v>0.1</v>
       </c>
       <c r="Q14" s="3" t="s">
@@ -2680,7 +2680,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
@@ -2692,19 +2692,19 @@
         <v>29</v>
       </c>
       <c r="F15" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>0.2</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="J15" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>29</v>
@@ -2716,7 +2716,7 @@
         <v>29</v>
       </c>
       <c r="N15" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>29</v>
@@ -2736,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3108,7 +3108,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -3120,7 +3120,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>15</v>
@@ -3132,7 +3132,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -3144,7 +3144,7 @@
         <v>15</v>
       </c>
       <c r="N8" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>15</v>
@@ -3161,7 +3161,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>29</v>
@@ -3173,7 +3173,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>29</v>
@@ -3185,7 +3185,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>29</v>
@@ -3197,7 +3197,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>29</v>
@@ -3270,52 +3270,52 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J11" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="L11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="P11" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>33</v>
@@ -3353,21 +3353,21 @@
       <c r="I12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="6">
         <f t="shared" si="0"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="6">
         <f t="shared" si="0"/>
         <v>0.69314718055994529</v>
       </c>
@@ -3414,14 +3414,14 @@
       <c r="I13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="9">
         <f>(3.5/75)^-0.25*N13</f>
         <v>2.0712917213851895E-2</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="9">
         <f>(3.5/75)^-0.25*P13</f>
         <v>2.0712917213851895E-2</v>
       </c>
@@ -3475,21 +3475,21 @@
       <c r="I14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="6">
         <f>(3.5/75)^-0.25*N14</f>
         <v>0.10356458606925947</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="6">
         <f>(3.5/75)^-0.25*P14</f>
         <v>0.10356458606925947</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <f>P14</f>
         <v>4.8135220872218422E-2</v>
       </c>
@@ -3506,59 +3506,56 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="L15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N15" s="5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="P15" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3566,893 +3563,973 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D461711-106C-4DEE-9CBC-A04E17BA8C3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="12" t="s">
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="5">
         <v>0</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="5">
         <v>0</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="5">
         <v>0</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="5">
         <v>0</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="5">
         <v>0</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="5">
         <v>2.5</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.05</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.04</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5">
         <v>1.5</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="14">
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="14">
-        <v>1</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="14">
+      <c r="M4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="5">
         <v>0.01</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="Q5" s="15" t="s">
+      <c r="B5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="5">
         <v>40</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="8">
         <v>40</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="7">
         <v>2</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="8">
         <v>40</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="5">
         <v>150</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="5">
         <v>3000</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="5">
+        <f>B6</f>
         <v>2</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:Q7" si="0">C6</f>
+        <v>L/kg</v>
+      </c>
+      <c r="D7" s="5">
         <v>40</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="14">
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>mL/kg</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="14">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>L/kg</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>mL/kg</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="14">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>L/kg</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="14">
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>mL/kg</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="O7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" s="14">
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>L</v>
+      </c>
+      <c r="P7" s="5">
         <v>3000</v>
       </c>
-      <c r="Q7" s="11" t="s">
-        <v>22</v>
+      <c r="Q7" t="str">
+        <f t="shared" si="0"/>
+        <v>mL</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="5">
+        <f>'1cmpt_PK_Model'!B7</f>
         <v>540</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="14">
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5">
+        <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="6">
+        <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="5">
+        <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="14">
+      <c r="K8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="6">
+        <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="14">
+      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="5">
+        <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="7">
+        <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="Q8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="5">
+        <f>B8*5</f>
         <v>2700</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1.8</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="C9" t="str">
+        <f t="shared" ref="C9:Q9" si="1">C8</f>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="D9" s="8">
+        <f>D8*5</f>
+        <v>1.75</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="F9" s="5">
+        <f>F8*5</f>
         <v>1650</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="H9" s="7">
+        <f>H8*5</f>
         <v>2</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="14">
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="J9" s="5">
+        <f>J8*5</f>
         <v>1300</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="14">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="L9" s="6">
+        <f>L8*5</f>
         <v>1.25</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="14">
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h/kg</v>
+      </c>
+      <c r="N9" s="5">
+        <f>N8*5</f>
         <v>50</v>
       </c>
-      <c r="O9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="14">
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>L/h</v>
+      </c>
+      <c r="P9" s="5">
+        <f>P8*5</f>
         <v>40</v>
       </c>
-      <c r="Q9" s="11" t="s">
-        <v>21</v>
+      <c r="Q9" t="str">
+        <f t="shared" si="1"/>
+        <v>mL/h</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5">
         <v>0.1</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5">
         <v>0.1</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="5">
         <v>0.1</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="M10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="5">
         <v>0.1</v>
       </c>
-      <c r="I10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="B11" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5">
         <v>0.2</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="16">
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="4">
         <v>0.2</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="14">
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="5">
         <v>0.2</v>
       </c>
-      <c r="M11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="14">
+      <c r="M11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="5">
         <v>0.2</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="14">
-        <v>1</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="14">
-        <v>1</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="14">
-        <v>1</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="14">
-        <v>1</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="15" t="s">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="5">
+        <f>F12</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5">
+        <f>H12</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="5">
+        <f>J12</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="5">
+        <f>L12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="5">
+        <f>N12</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="5">
+        <f>P12</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="7">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="5">
+        <v>10000</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6">
+        <f>LN(2)/1</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="6">
+        <f>LN(2)/1</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:N14" si="2">H14</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="6">
+        <f>LN(2)/1</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="9">
+        <f>(0.025/75)^-0.25*N15</f>
+        <v>7.1248098515933986E-2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9">
+        <f>(0.025/75)^-0.25*P15</f>
+        <v>7.1248098515933986E-2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="9">
+        <f>(0.25/75)^-0.25*N15</f>
+        <v>4.0065750136742871E-2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="9">
+        <f>(0.25/75)^-0.25*P15</f>
+        <v>4.0065750136742871E-2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="9">
+        <f>(3.5/75)^-0.25*N15</f>
+        <v>2.0712917213851895E-2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9">
+        <f>(3.5/75)^-0.25*P15</f>
+        <v>2.0712917213851895E-2</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="10">
+        <f>P15</f>
+        <v>9.6270441744436847E-3</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="10">
+        <f>LN(2)/72</f>
+        <v>9.6270441744436847E-3</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6">
+        <f>(0.025/75)^-0.25*N16</f>
+        <v>0.35624049257966989</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6">
+        <f>(0.025/75)^-0.25*P16</f>
+        <v>0.35624049257966989</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="6">
+        <f>(0.25/75)^-0.25*N16</f>
+        <v>0.20032875068371434</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="6">
+        <f>(0.25/75)^-0.25*P16</f>
+        <v>0.20032875068371434</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="6">
+        <f>(3.5/75)^-0.25*N16</f>
+        <v>0.10356458606925947</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="6">
+        <f>(3.5/75)^-0.25*P16</f>
+        <v>0.10356458606925947</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="9">
+        <f>P16</f>
+        <v>4.8135220872218422E-2</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="10">
+        <f>P15*5</f>
+        <v>4.8135220872218422E-2</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="Q13" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="14">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0.69314718099999995</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="14">
-        <v>0.69314718099999995</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N14" s="14">
-        <v>0.69314718099999995</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P14" s="14">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="Q14" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="14">
-        <v>7.1199999999999999E-2</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="14">
-        <v>7.1199999999999999E-2</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="14">
-        <v>4.0099999999999997E-2</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="14">
-        <v>4.0099999999999997E-2</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="14">
-        <v>2.0712917000000001E-2</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="14">
-        <v>2.0712917000000001E-2</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="14">
-        <v>9.6299999999999997E-3</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P15" s="14">
-        <v>9.6299999999999997E-3</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="14">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="14">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="14">
-        <v>0.103564586</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" s="14">
-        <v>0.103564586</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N16" s="14">
-        <v>4.8140000000000002E-2</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P16" s="14">
-        <v>4.8140000000000002E-2</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="Q17" s="15" t="s">
+      <c r="B17" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1000</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="5">
+        <v>10000</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add per-body-weight option
</commit_message>
<xml_diff>
--- a/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
+++ b/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrobins/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33D707-3E5B-4E65-8A27-8A59E25C8062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BD4D42-8CA2-E041-B7EB-9ECB6257AF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cmpt_PK_Model" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="40">
   <si>
     <t>SM_Mouse</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>L/kg</t>
-  </si>
-  <si>
-    <t>mL/h/kg</t>
   </si>
   <si>
     <t>L/h</t>
@@ -530,30 +527,30 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" activeCellId="1" sqref="A8:XFD8 A9:XFD9"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,10 +558,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -579,57 +576,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -682,7 +679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -735,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -743,52 +740,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -796,37 +793,37 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4">
         <v>80</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5">
         <v>80</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>300</v>
@@ -838,10 +835,10 @@
         <v>6000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -849,166 +846,166 @@
         <v>540</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
         <v>0.35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5">
         <v>330</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <v>0.4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="5">
         <v>260</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" s="7">
         <v>0.25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="5">
         <v>10</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5">
         <v>8</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5">
         <f>B7</f>
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="5">
         <f>H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="5">
         <f>L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="5">
         <f>P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5">
         <v>1000</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5">
         <v>1000</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" s="5">
         <v>1000</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="7">
         <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N9" s="5">
         <v>1000</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P9" s="7">
         <v>1</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1061,57 +1058,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5">
         <v>0.02</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5">
         <v>0.2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <v>0.02</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4">
         <v>0.2</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="5">
         <v>0.02</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5">
         <v>0.2</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N11" s="5">
         <v>0.02</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" s="5">
         <v>0.2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1125,30 +1122,30 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1156,10 +1153,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1174,57 +1171,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1338,52 +1335,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1391,37 +1388,37 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -1433,12 +1430,12 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <f>B6</f>
@@ -1446,14 +1443,14 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q7" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -1461,7 +1458,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -1469,7 +1466,7 @@
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
@@ -1477,7 +1474,7 @@
       </c>
       <c r="K7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
@@ -1485,7 +1482,7 @@
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -1503,7 +1500,7 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1512,61 +1509,61 @@
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <f>B8*5</f>
@@ -1574,7 +1571,7 @@
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" ref="C9:Q9" si="1">C8</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D9" s="8">
         <f>D8*5</f>
@@ -1582,7 +1579,7 @@
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F9" s="5">
         <f>F8*5</f>
@@ -1590,7 +1587,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H9" s="7">
         <f>H8*5</f>
@@ -1598,7 +1595,7 @@
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J9" s="5">
         <f>J8*5</f>
@@ -1606,7 +1603,7 @@
       </c>
       <c r="K9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L9" s="6">
         <f>L8*5</f>
@@ -1614,7 +1611,7 @@
       </c>
       <c r="M9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N9" s="5">
         <f>N8*5</f>
@@ -1633,121 +1630,121 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5">
         <f>B8</f>
         <v>540</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5">
         <f>D8</f>
         <v>0.35</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5">
         <f>F8</f>
         <v>330</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5">
         <f>H8</f>
         <v>0.4</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="5">
         <f>J8</f>
         <v>260</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L10" s="5">
         <f>L8</f>
         <v>0.25</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" s="5">
         <f>N8</f>
         <v>10</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P10" s="5">
         <f>P8</f>
         <v>8</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5">
         <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5">
         <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="5">
         <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="5">
         <v>1000</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P11" s="7">
         <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,57 +1797,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5">
         <v>0.02</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5">
         <v>0.2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="5">
         <v>0.02</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="4">
         <v>0.2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="5">
         <v>0.02</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L13" s="5">
         <v>0.2</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N13" s="5">
         <v>0.02</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P13" s="5">
         <v>0.2</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1864,30 +1861,30 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1895,10 +1892,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1913,57 +1910,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2077,52 +2074,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2130,19 +2127,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
@@ -2160,7 +2157,7 @@
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -2172,26 +2169,26 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q8" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -2199,7 +2196,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -2223,7 +2220,7 @@
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -2241,9 +2238,9 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5">
         <f>B7/2</f>
@@ -2251,7 +2248,7 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D8" s="5">
         <f>D7/2</f>
@@ -2259,7 +2256,7 @@
       </c>
       <c r="E8" s="3" t="str">
         <f>E7</f>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F8" s="5">
         <f>F7/2</f>
@@ -2267,7 +2264,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f>G7</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H8" s="5">
         <f>H7/2</f>
@@ -2291,7 +2288,7 @@
       </c>
       <c r="M8" s="3" t="str">
         <f>M7</f>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N8" s="5">
         <f>N7/2</f>
@@ -2306,10 +2303,10 @@
         <v>1500</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2318,61 +2315,61 @@
         <v>540</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L9" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N9" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <f>B9*5</f>
@@ -2380,7 +2377,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" ref="C10:Q11" si="1">C9</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D10" s="8">
         <f>D9*5</f>
@@ -2388,7 +2385,7 @@
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F10" s="5">
         <f>F9*5</f>
@@ -2396,7 +2393,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H10" s="7">
         <f>H9*5</f>
@@ -2404,7 +2401,7 @@
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J10" s="5">
         <f>J9*5</f>
@@ -2412,7 +2409,7 @@
       </c>
       <c r="K10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L10" s="6">
         <f>L9*5</f>
@@ -2420,7 +2417,7 @@
       </c>
       <c r="M10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N10" s="5">
         <f>N9*5</f>
@@ -2439,9 +2436,9 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5">
         <f>B10/50</f>
@@ -2449,7 +2446,7 @@
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D11" s="5">
         <f>D10/50</f>
@@ -2457,7 +2454,7 @@
       </c>
       <c r="E11" s="3" t="str">
         <f>E10</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F11" s="5">
         <f>F10/50</f>
@@ -2465,7 +2462,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H11" s="5">
         <f>H10/50</f>
@@ -2473,7 +2470,7 @@
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J11" s="5">
         <f>J10/50</f>
@@ -2481,7 +2478,7 @@
       </c>
       <c r="K11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L11" s="5">
         <f>L10/50</f>
@@ -2489,7 +2486,7 @@
       </c>
       <c r="M11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N11" s="5">
         <f>N10/50</f>
@@ -2508,121 +2505,121 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5">
         <f>B9</f>
         <v>540</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5">
         <f>D9</f>
         <v>0.35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5">
         <f>F9</f>
         <v>330</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" s="5">
         <f>H9</f>
         <v>0.4</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="5">
         <f>J9</f>
         <v>260</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L12" s="5">
         <f>L9</f>
         <v>0.25</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N12" s="5">
         <f>N9</f>
         <v>10</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" s="5">
         <f>P9</f>
         <v>8</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5">
         <v>1000</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5">
         <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="5">
         <v>1000</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="7">
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="5">
         <v>1000</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P13" s="7">
         <v>1</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2675,57 +2672,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5">
         <v>0.02</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5">
         <v>0.2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="5">
         <v>0.02</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="4">
         <v>0.2</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="5">
         <v>0.02</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L15" s="5">
         <v>0.2</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N15" s="5">
         <v>0.02</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P15" s="5">
         <v>0.2</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2739,30 +2736,30 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2770,10 +2767,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -2788,57 +2785,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2891,7 +2888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2952,52 +2949,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3005,37 +3002,37 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4">
         <v>80</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5">
         <v>80</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>300</v>
@@ -3047,10 +3044,10 @@
         <v>6000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -3058,52 +3055,52 @@
         <v>540</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
         <v>0.35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5">
         <v>330</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <v>0.4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="5">
         <v>260</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" s="7">
         <v>0.25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="5">
         <v>10</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5">
         <v>8</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3156,7 +3153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3164,166 +3161,166 @@
         <v>0.02</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="5">
         <v>0.2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5">
         <v>0.02</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4">
         <v>0.2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="5">
         <v>0.02</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" s="5">
         <v>0.2</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="5">
         <v>0.02</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P9" s="5">
         <v>0.2</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5">
         <f>F10</f>
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="5">
         <f>H10</f>
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="5">
         <f>J10</f>
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="5">
         <f>L10</f>
         <v>1</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L10" s="5">
         <f>N10</f>
         <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" s="5">
         <f>P10</f>
         <v>1</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P10" s="5">
         <v>1</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5">
         <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5">
         <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="5">
         <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="5">
         <v>10000</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P11" s="7">
         <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6">
         <f>LN(2)/1</f>
@@ -3382,9 +3379,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="9">
         <f>(0.025/75)^-0.25*N13</f>
@@ -3443,9 +3440,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="6">
         <f>(0.025/75)^-0.25*N14</f>
@@ -3504,163 +3501,163 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5">
         <v>1000</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="5">
         <v>1000</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7">
         <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="5">
         <v>1000</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L15" s="7">
         <v>1</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" s="5">
         <v>10000</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P15" s="7">
         <v>1</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5">
         <v>540</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5">
         <v>0.35</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5">
         <v>330</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="5">
         <v>0.4</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="5">
         <v>260</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L16" s="5">
         <v>0.25</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N16" s="5">
         <v>10</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" s="5">
         <v>8</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5">
         <v>1000</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5">
         <v>1000</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="5">
         <v>1000</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" s="7">
         <v>1</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="5">
         <v>1000</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3676,31 +3673,31 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3708,10 +3705,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -3726,57 +3723,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3829,7 +3826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -3882,7 +3879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3890,52 +3887,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3943,37 +3940,37 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -3985,12 +3982,12 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <f>B6</f>
@@ -3998,14 +3995,14 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:Q7" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -4013,7 +4010,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -4021,7 +4018,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
@@ -4029,7 +4026,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
@@ -4037,7 +4034,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -4055,7 +4052,7 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -4064,61 +4061,61 @@
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <f>B8*5</f>
@@ -4126,7 +4123,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" ref="C9:Q9" si="1">C8</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D9" s="8">
         <f>D8*5</f>
@@ -4134,7 +4131,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F9" s="5">
         <f>F8*5</f>
@@ -4142,7 +4139,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H9" s="7">
         <f>H8*5</f>
@@ -4150,7 +4147,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J9" s="5">
         <f>J8*5</f>
@@ -4158,7 +4155,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L9" s="6">
         <f>L8*5</f>
@@ -4166,7 +4163,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N9" s="5">
         <f>N8*5</f>
@@ -4185,7 +4182,7 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -4238,7 +4235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -4246,166 +4243,166 @@
         <v>0.02</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5">
         <v>0.2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <v>0.02</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4">
         <v>0.2</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="5">
         <v>0.02</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5">
         <v>0.2</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N11" s="5">
         <v>0.02</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" s="5">
         <v>0.2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5">
         <f>F12</f>
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5">
         <f>H12</f>
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="5">
         <f>J12</f>
         <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="5">
         <f>L12</f>
         <v>1</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L12" s="5">
         <f>N12</f>
         <v>1</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="5">
         <f>P12</f>
         <v>1</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P12" s="5">
         <v>1</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5">
         <v>1000</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5">
         <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="5">
         <v>1000</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="7">
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="5">
         <v>10000</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P13" s="7">
         <v>1</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6">
         <f>LN(2)/1</f>
@@ -4464,9 +4461,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="9">
         <f>(0.025/75)^-0.25*N15</f>
@@ -4525,9 +4522,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6">
         <f>(0.025/75)^-0.25*N16</f>
@@ -4586,171 +4583,171 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5">
         <v>1000</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5">
         <v>1000</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="5">
         <v>1000</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" s="7">
         <v>1</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="5">
         <v>10000</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5">
         <f>B8</f>
         <v>540</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="5">
         <f>D8</f>
         <v>0.35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5">
         <f>F8</f>
         <v>330</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H18" s="5">
         <f>H8</f>
         <v>0.4</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="5">
         <f>J8</f>
         <v>260</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L18" s="5">
         <f>L8</f>
         <v>0.25</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N18" s="5">
         <f>N8</f>
         <v>10</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P18" s="5">
         <f>P8</f>
         <v>8</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5">
         <v>1000</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="5">
         <v>1000</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="5">
         <v>1000</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" s="7">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="5">
         <v>1000</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P19" s="7">
         <v>1</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add per-body-weight options for dosing amounts and pk parameters (#885)
* feat: add per-body-weight option

* Update pkpdapp/pkpdapp/models/myokit_model_mixin.py

* Update pkpdapp/pkpdapp/models/myokit_model_mixin.py

* flake8

* fix tests
</commit_message>
<xml_diff>
--- a/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
+++ b/pkpdapp/pkpdapp/migrations/models/ParametersValue_Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrobins/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33D707-3E5B-4E65-8A27-8A59E25C8062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BD4D42-8CA2-E041-B7EB-9ECB6257AF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1cmpt_PK_Model" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="40">
   <si>
     <t>SM_Mouse</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>L/kg</t>
-  </si>
-  <si>
-    <t>mL/h/kg</t>
   </si>
   <si>
     <t>L/h</t>
@@ -530,30 +527,30 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" activeCellId="1" sqref="A8:XFD8 A9:XFD9"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,10 +558,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -579,57 +576,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -682,7 +679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -735,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -743,52 +740,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -796,37 +793,37 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4">
         <v>80</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5">
         <v>80</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>300</v>
@@ -838,10 +835,10 @@
         <v>6000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -849,166 +846,166 @@
         <v>540</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
         <v>0.35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5">
         <v>330</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <v>0.4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="5">
         <v>260</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" s="7">
         <v>0.25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="5">
         <v>10</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5">
         <v>8</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5">
         <f>B7</f>
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="5">
         <f>H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="5">
         <f>L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="5">
         <f>P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5">
         <v>1000</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5">
         <v>1000</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" s="5">
         <v>1000</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="7">
         <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N9" s="5">
         <v>1000</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P9" s="7">
         <v>1</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1061,57 +1058,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5">
         <v>0.02</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5">
         <v>0.2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <v>0.02</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4">
         <v>0.2</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="5">
         <v>0.02</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5">
         <v>0.2</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N11" s="5">
         <v>0.02</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" s="5">
         <v>0.2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1125,30 +1122,30 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1156,10 +1153,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1174,57 +1171,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1338,52 +1335,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1391,37 +1388,37 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -1433,12 +1430,12 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <f>B6</f>
@@ -1446,14 +1443,14 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q7" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -1461,7 +1458,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -1469,7 +1466,7 @@
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
@@ -1477,7 +1474,7 @@
       </c>
       <c r="K7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
@@ -1485,7 +1482,7 @@
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -1503,7 +1500,7 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1512,61 +1509,61 @@
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <f>B8*5</f>
@@ -1574,7 +1571,7 @@
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" ref="C9:Q9" si="1">C8</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D9" s="8">
         <f>D8*5</f>
@@ -1582,7 +1579,7 @@
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F9" s="5">
         <f>F8*5</f>
@@ -1590,7 +1587,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H9" s="7">
         <f>H8*5</f>
@@ -1598,7 +1595,7 @@
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J9" s="5">
         <f>J8*5</f>
@@ -1606,7 +1603,7 @@
       </c>
       <c r="K9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L9" s="6">
         <f>L8*5</f>
@@ -1614,7 +1611,7 @@
       </c>
       <c r="M9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N9" s="5">
         <f>N8*5</f>
@@ -1633,121 +1630,121 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5">
         <f>B8</f>
         <v>540</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5">
         <f>D8</f>
         <v>0.35</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5">
         <f>F8</f>
         <v>330</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5">
         <f>H8</f>
         <v>0.4</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="5">
         <f>J8</f>
         <v>260</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L10" s="5">
         <f>L8</f>
         <v>0.25</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" s="5">
         <f>N8</f>
         <v>10</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P10" s="5">
         <f>P8</f>
         <v>8</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5">
         <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5">
         <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="5">
         <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="5">
         <v>1000</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P11" s="7">
         <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,57 +1797,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5">
         <v>0.02</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5">
         <v>0.2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="5">
         <v>0.02</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="4">
         <v>0.2</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="5">
         <v>0.02</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L13" s="5">
         <v>0.2</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N13" s="5">
         <v>0.02</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P13" s="5">
         <v>0.2</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1864,30 +1861,30 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1895,10 +1892,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1913,57 +1910,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2077,52 +2074,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2130,19 +2127,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
@@ -2160,7 +2157,7 @@
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -2172,26 +2169,26 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:Q8" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -2199,7 +2196,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -2223,7 +2220,7 @@
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -2241,9 +2238,9 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5">
         <f>B7/2</f>
@@ -2251,7 +2248,7 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D8" s="5">
         <f>D7/2</f>
@@ -2259,7 +2256,7 @@
       </c>
       <c r="E8" s="3" t="str">
         <f>E7</f>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F8" s="5">
         <f>F7/2</f>
@@ -2267,7 +2264,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f>G7</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H8" s="5">
         <f>H7/2</f>
@@ -2291,7 +2288,7 @@
       </c>
       <c r="M8" s="3" t="str">
         <f>M7</f>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N8" s="5">
         <f>N7/2</f>
@@ -2306,10 +2303,10 @@
         <v>1500</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2318,61 +2315,61 @@
         <v>540</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L9" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N9" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <f>B9*5</f>
@@ -2380,7 +2377,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" ref="C10:Q11" si="1">C9</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D10" s="8">
         <f>D9*5</f>
@@ -2388,7 +2385,7 @@
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F10" s="5">
         <f>F9*5</f>
@@ -2396,7 +2393,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H10" s="7">
         <f>H9*5</f>
@@ -2404,7 +2401,7 @@
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J10" s="5">
         <f>J9*5</f>
@@ -2412,7 +2409,7 @@
       </c>
       <c r="K10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L10" s="6">
         <f>L9*5</f>
@@ -2420,7 +2417,7 @@
       </c>
       <c r="M10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N10" s="5">
         <f>N9*5</f>
@@ -2439,9 +2436,9 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5">
         <f>B10/50</f>
@@ -2449,7 +2446,7 @@
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D11" s="5">
         <f>D10/50</f>
@@ -2457,7 +2454,7 @@
       </c>
       <c r="E11" s="3" t="str">
         <f>E10</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F11" s="5">
         <f>F10/50</f>
@@ -2465,7 +2462,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H11" s="5">
         <f>H10/50</f>
@@ -2473,7 +2470,7 @@
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J11" s="5">
         <f>J10/50</f>
@@ -2481,7 +2478,7 @@
       </c>
       <c r="K11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L11" s="5">
         <f>L10/50</f>
@@ -2489,7 +2486,7 @@
       </c>
       <c r="M11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N11" s="5">
         <f>N10/50</f>
@@ -2508,121 +2505,121 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5">
         <f>B9</f>
         <v>540</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5">
         <f>D9</f>
         <v>0.35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5">
         <f>F9</f>
         <v>330</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" s="5">
         <f>H9</f>
         <v>0.4</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="5">
         <f>J9</f>
         <v>260</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L12" s="5">
         <f>L9</f>
         <v>0.25</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N12" s="5">
         <f>N9</f>
         <v>10</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" s="5">
         <f>P9</f>
         <v>8</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5">
         <v>1000</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5">
         <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="5">
         <v>1000</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="7">
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="5">
         <v>1000</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P13" s="7">
         <v>1</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2675,57 +2672,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5">
         <v>0.02</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5">
         <v>0.2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="5">
         <v>0.02</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="4">
         <v>0.2</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="5">
         <v>0.02</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L15" s="5">
         <v>0.2</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N15" s="5">
         <v>0.02</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P15" s="5">
         <v>0.2</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2739,30 +2736,30 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2770,10 +2767,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -2788,57 +2785,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2891,7 +2888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2952,52 +2949,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3005,37 +3002,37 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4">
         <v>80</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5">
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5">
         <v>80</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>300</v>
@@ -3047,10 +3044,10 @@
         <v>6000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -3058,52 +3055,52 @@
         <v>540</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
         <v>0.35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5">
         <v>330</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <v>0.4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="5">
         <v>260</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" s="7">
         <v>0.25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="5">
         <v>10</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5">
         <v>8</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3156,7 +3153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3164,166 +3161,166 @@
         <v>0.02</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="5">
         <v>0.2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5">
         <v>0.02</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4">
         <v>0.2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="5">
         <v>0.02</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" s="5">
         <v>0.2</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="5">
         <v>0.02</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P9" s="5">
         <v>0.2</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5">
         <f>F10</f>
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="5">
         <f>H10</f>
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="5">
         <f>J10</f>
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="5">
         <f>L10</f>
         <v>1</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L10" s="5">
         <f>N10</f>
         <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" s="5">
         <f>P10</f>
         <v>1</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P10" s="5">
         <v>1</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5">
         <v>1000</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5">
         <v>1000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="5">
         <v>1000</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="5">
         <v>10000</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P11" s="7">
         <v>1</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6">
         <f>LN(2)/1</f>
@@ -3382,9 +3379,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="9">
         <f>(0.025/75)^-0.25*N13</f>
@@ -3443,9 +3440,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="6">
         <f>(0.025/75)^-0.25*N14</f>
@@ -3504,163 +3501,163 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5">
         <v>1000</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="5">
         <v>1000</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7">
         <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="5">
         <v>1000</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L15" s="7">
         <v>1</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" s="5">
         <v>10000</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P15" s="7">
         <v>1</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5">
         <v>540</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5">
         <v>0.35</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5">
         <v>330</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="5">
         <v>0.4</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="5">
         <v>260</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L16" s="5">
         <v>0.25</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N16" s="5">
         <v>10</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" s="5">
         <v>8</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5">
         <v>1000</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5">
         <v>1000</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="5">
         <v>1000</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" s="7">
         <v>1</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="5">
         <v>1000</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3676,31 +3673,31 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3708,10 +3705,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -3726,57 +3723,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3829,7 +3826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -3882,7 +3879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3890,52 +3887,52 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5">
         <v>0.5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5">
         <v>0.5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="5">
         <v>0.5</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="5">
         <v>0.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.5</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5">
         <v>0.5</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3943,37 +3940,37 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8">
         <v>40</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>40</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5">
         <v>150</v>
@@ -3985,12 +3982,12 @@
         <v>3000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <f>B6</f>
@@ -3998,14 +3995,14 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:Q7" si="0">C6</f>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -4013,7 +4010,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
@@ -4021,7 +4018,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
@@ -4029,7 +4026,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>L/kg</v>
+        <v>L</v>
       </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
@@ -4037,7 +4034,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>mL/kg</v>
+        <v>mL</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
@@ -4055,7 +4052,7 @@
         <v>mL</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -4064,61 +4061,61 @@
         <v>540</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f>'1cmpt_PK_Model'!D7</f>
         <v>0.35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5">
         <f>'1cmpt_PK_Model'!F7</f>
         <v>330</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6">
         <f>'1cmpt_PK_Model'!H7</f>
         <v>0.4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5">
         <f>'1cmpt_PK_Model'!J7</f>
         <v>260</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="6">
         <f>'1cmpt_PK_Model'!L7</f>
         <v>0.25</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="5">
         <f>'1cmpt_PK_Model'!N7</f>
         <v>10</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="7">
         <f>'1cmpt_PK_Model'!P7</f>
         <v>8</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <f>B8*5</f>
@@ -4126,7 +4123,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" ref="C9:Q9" si="1">C8</f>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="D9" s="8">
         <f>D8*5</f>
@@ -4134,7 +4131,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="F9" s="5">
         <f>F8*5</f>
@@ -4142,7 +4139,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="H9" s="7">
         <f>H8*5</f>
@@ -4150,7 +4147,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="J9" s="5">
         <f>J8*5</f>
@@ -4158,7 +4155,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="L9" s="6">
         <f>L8*5</f>
@@ -4166,7 +4163,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>mL/h/kg</v>
+        <v>mL/h</v>
       </c>
       <c r="N9" s="5">
         <f>N8*5</f>
@@ -4185,7 +4182,7 @@
         <v>mL/h</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -4238,7 +4235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -4246,166 +4243,166 @@
         <v>0.02</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5">
         <v>0.2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <v>0.02</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4">
         <v>0.2</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="5">
         <v>0.02</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5">
         <v>0.2</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N11" s="5">
         <v>0.02</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" s="5">
         <v>0.2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5">
         <f>F12</f>
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5">
         <f>H12</f>
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="5">
         <f>J12</f>
         <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="5">
         <f>L12</f>
         <v>1</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L12" s="5">
         <f>N12</f>
         <v>1</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="5">
         <f>P12</f>
         <v>1</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P12" s="5">
         <v>1</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5">
         <v>1000</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5">
         <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="5">
         <v>1000</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="7">
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="5">
         <v>10000</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P13" s="7">
         <v>1</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6">
         <f>LN(2)/1</f>
@@ -4464,9 +4461,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="9">
         <f>(0.025/75)^-0.25*N15</f>
@@ -4525,9 +4522,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6">
         <f>(0.025/75)^-0.25*N16</f>
@@ -4586,171 +4583,171 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5">
         <v>1000</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5">
         <v>1000</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="5">
         <v>1000</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" s="7">
         <v>1</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="5">
         <v>10000</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5">
         <f>B8</f>
         <v>540</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="5">
         <f>D8</f>
         <v>0.35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5">
         <f>F8</f>
         <v>330</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H18" s="5">
         <f>H8</f>
         <v>0.4</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="5">
         <f>J8</f>
         <v>260</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L18" s="5">
         <f>L8</f>
         <v>0.25</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N18" s="5">
         <f>N8</f>
         <v>10</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P18" s="5">
         <f>P8</f>
         <v>8</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5">
         <v>1000</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="5">
         <v>1000</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="5">
         <v>1000</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" s="7">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="5">
         <v>1000</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P19" s="7">
         <v>1</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>